<commit_message>
Tidied up simulation - N partitioning plot to go
</commit_message>
<xml_diff>
--- a/Tests/Simulation/SoilNitrogenPatch/N for Pregnancy.xlsx
+++ b/Tests/Simulation/SoilNitrogenPatch/N for Pregnancy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaUnderVC\ApsimX\Tests\Simulation\SoilNitrogenPatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70BC5EF-D4AE-4D7B-B6C5-EBBA8738A802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853D1538-F263-4585-AAAF-D02B7BC165F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="1350" windowWidth="29655" windowHeight="18525" xr2:uid="{0CEA60F6-DC99-4D2D-8C90-8D88CAF277DA}"/>
+    <workbookView xWindow="990" yWindow="1785" windowWidth="20715" windowHeight="18525" xr2:uid="{0CEA60F6-DC99-4D2D-8C90-8D88CAF277DA}"/>
   </bookViews>
   <sheets>
     <sheet name="ARC from Robyn" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +143,14 @@
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,9 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,9 +209,49 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.7692038495188095E-2"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.90297462817147855"/>
+          <c:h val="0.84204505686789155"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -210,11 +260,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ARC from Robyn'!$C$7</c:f>
+              <c:f>'ARC from Robyn'!$J$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pr Calf</c:v>
+                  <c:v>N by day</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -374,129 +424,129 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ARC from Robyn'!$C$8:$C$47</c:f>
+              <c:f>'ARC from Robyn'!$J$8:$J$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>6.801222499401326E-5</c:v>
+                  <c:v>1.2978900663845563E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1694963390665244E-4</c:v>
+                  <c:v>1.5835620917430349E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9711061015858003E-4</c:v>
+                  <c:v>1.925241984737405E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2586818873865859E-4</c:v>
+                  <c:v>2.332791948207497E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2881583501794484E-4</c:v>
+                  <c:v>2.8177051251740312E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4293813413467136E-4</c:v>
+                  <c:v>3.39337037352202E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3206962350561075E-3</c:v>
+                  <c:v>4.0753705952118044E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.035179749598973E-3</c:v>
+                  <c:v>4.8818122659795711E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0864666142974592E-3</c:v>
+                  <c:v>5.8336810159858113E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.6093099255578628E-3</c:v>
+                  <c:v>6.9552149298062599E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.7822346306760008E-3</c:v>
+                  <c:v>8.2742838542028462E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.8380767700469163E-3</c:v>
+                  <c:v>9.82275966790186E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.4075934382809088E-2</c:v>
+                  <c:v>1.1636859459871853E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9874424073124966E-2</c:v>
+                  <c:v>1.3757441174869476E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7706053649323156E-2</c:v>
+                  <c:v>1.6230229795484183E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8152433331449742E-2</c:v>
+                  <c:v>1.9105951772573366E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1919960751586745E-2</c:v>
+                  <c:v>2.2440356354628791E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.9855533827244479E-2</c:v>
+                  <c:v>2.6294104774668308E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.2961776155498846E-2</c:v>
+                  <c:v>3.0732511901911648E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12241120710999331</c:v>
+                  <c:v>3.5825129821698636E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1595587578323498</c:v>
+                  <c:v>4.1645168641356598E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.20595202818678859</c:v>
+                  <c:v>4.8268756323067239E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.26333870048840585</c:v>
+                  <c:v>5.5774046152854521E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.3336705738508271</c:v>
+                  <c:v>6.4240187176447926E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.4191037571419699</c:v>
+                  <c:v>7.3746179180147519E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.52199465606193418</c:v>
+                  <c:v>8.4369639212314423E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.64489150668751249</c:v>
+                  <c:v>9.6185510930240376E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.79052133881471387</c:v>
+                  <c:v>1.0926475099558493E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.96177239169730955</c:v>
+                  <c:v>1.2367302819512154E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.1616721460996831</c:v>
+                  <c:v>1.3946947089055577E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3933612737606456</c:v>
+                  <c:v>1.5670549684976696E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6600639325924096</c:v>
+                  <c:v>1.7542375661073233E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.9650549480984005</c:v>
+                  <c:v>1.9565721747398034E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3116245144007945</c:v>
+                  <c:v>2.1742841025438685E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.703041118834955</c:v>
+                  <c:v>2.4074885532350921E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.1425134403857591</c:v>
+                  <c:v>2.6561867852598224E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.6331519935904493</c:v>
+                  <c:v>2.9202642153817512E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.1779312863227629</c:v>
+                  <c:v>3.1994904541348908E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.7796532335225521</c:v>
+                  <c:v>3.4935212065233617E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.440912521714206</c:v>
+                  <c:v>3.8019019233025225E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,309 +555,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2059-463B-92A8-F4035E64D925}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ARC from Robyn'!$D$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pr Uterus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'ARC from Robyn'!$A$8:$A$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'ARC from Robyn'!$D$8:$D$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
-                <c:pt idx="0">
-                  <c:v>9.7230654201753142E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2287663178814686E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5462788886750765E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.9377260065973095E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4183318083505614E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.0060122989741526E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7217632310038634E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.5900884270609579E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.6394703854019748E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.9028847475679306E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.4183598939493787E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.10229582566649324</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.12386550000295146</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.14946268572300453</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.17973498467474197</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.21541543291884618</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.25733082972662075</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.3064104765016652</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.36369529613816781</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.43034729660938909</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.50765933578049882</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.59706513765502311</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.70014950359276529</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.81865865558148732</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.95451064250799922</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.1098057346592547</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.286836726490596</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.4880990631216289</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.7163007021495973</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.9743716192863507</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.2654728640994213</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.5930050708304533</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.9606163289232574</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.3722093185537796</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.831947618135997</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.3442610934874448</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4.9138502820679975</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>5.5456896904322104</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.2450299287233157</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7.0173986126343495</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2059-463B-92A8-F4035E64D925}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1192,124 +939,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>6.801222499401326E-5</c:v>
+                  <c:v>7.1412836243713924E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1694963390665244E-4</c:v>
+                  <c:v>1.2279711560198505E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9711061015858003E-4</c:v>
+                  <c:v>2.0696614066650904E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2586818873865859E-4</c:v>
+                  <c:v>3.4216159817559153E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2881583501794484E-4</c:v>
+                  <c:v>5.5525662676884208E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4293813413467136E-4</c:v>
+                  <c:v>8.8508504084140499E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3206962350561075E-3</c:v>
+                  <c:v>1.3867310468089129E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.035179749598973E-3</c:v>
+                  <c:v>2.1369387370789215E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0864666142974592E-3</c:v>
+                  <c:v>3.2407899450123323E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.6093099255578628E-3</c:v>
+                  <c:v>4.8397754218357557E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.7822346306760008E-3</c:v>
+                  <c:v>7.121346362209801E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.8380767700469163E-3</c:v>
+                  <c:v>1.0329980608549262E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.4075934382809088E-2</c:v>
+                  <c:v>1.4779731101949542E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9874424073124966E-2</c:v>
+                  <c:v>2.0868145276781214E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7706053649323156E-2</c:v>
+                  <c:v>2.9091356331789314E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8152433331449742E-2</c:v>
+                  <c:v>4.0060054998022232E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1919960751586745E-2</c:v>
+                  <c:v>5.4515958789166083E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.9855533827244479E-2</c:v>
+                  <c:v>7.3348310518606699E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.2961776155498846E-2</c:v>
+                  <c:v>9.7609864963273785E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12241120710999331</c:v>
+                  <c:v>0.12853176746549297</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1595587578323498</c:v>
+                  <c:v>0.16753669572396726</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.20595202818678859</c:v>
+                  <c:v>0.21624962959612803</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.26333870048840585</c:v>
+                  <c:v>0.27650563551282614</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.3336705738508271</c:v>
+                  <c:v>0.35035410254336841</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.4191037571419699</c:v>
+                  <c:v>0.44005894499906839</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.52199465606193418</c:v>
+                  <c:v>0.54809438886503081</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.64489150668751249</c:v>
+                  <c:v>0.67713608202188813</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.79052133881471387</c:v>
+                  <c:v>0.83004740575544955</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.96177239169730955</c:v>
+                  <c:v>1.0098610112821749</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.1616721460996831</c:v>
+                  <c:v>1.2197557534046672</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3933612737606456</c:v>
+                  <c:v>1.4630293374486778</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6600639325924096</c:v>
+                  <c:v>1.7430671292220299</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.9650549480984005</c:v>
+                  <c:v>2.0633076955033203</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3116245144007945</c:v>
+                  <c:v>2.4272057401208342</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.703041118834955</c:v>
+                  <c:v>2.8381931747767029</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.1425134403857591</c:v>
+                  <c:v>3.299639112405047</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.6331519935904493</c:v>
+                  <c:v>3.8148095932699717</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.1779312863227629</c:v>
+                  <c:v>4.3868278506389009</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.7796532335225521</c:v>
+                  <c:v>5.0186358951986803</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.440912521714206</c:v>
+                  <c:v>5.7129581477999158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,124 +1242,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>9.7230654201753142E-3</c:v>
+                  <c:v>1.020921869118408E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2287663178814686E-2</c:v>
+                  <c:v>1.2902046337755421E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5462788886750765E-2</c:v>
+                  <c:v>1.6235928331088303E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9377260065973095E-2</c:v>
+                  <c:v>2.0346123069271749E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4183318083505614E-2</c:v>
+                  <c:v>2.5392483987680896E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0060122989741526E-2</c:v>
+                  <c:v>3.1563129139228603E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.7217632310038634E-2</c:v>
+                  <c:v>3.9078513925540563E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5900884270609579E-2</c:v>
+                  <c:v>4.8195928484140053E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.6394703854019748E-2</c:v>
+                  <c:v>5.9214439046720739E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9028847475679306E-2</c:v>
+                  <c:v>7.2480289849463267E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.4183598939493787E-2</c:v>
+                  <c:v>8.8392778886468473E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10229582566649324</c:v>
+                  <c:v>0.10741061694981791</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.12386550000295146</c:v>
+                  <c:v>0.13005877500309904</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.14946268572300453</c:v>
+                  <c:v>0.15693582000915474</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.17973498467474197</c:v>
+                  <c:v>0.18872173390847907</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.21541543291884618</c:v>
+                  <c:v>0.22618620456478847</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25733082972662075</c:v>
+                  <c:v>0.27019737121295179</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.3064104765016652</c:v>
+                  <c:v>0.3217310003267484</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.36369529613816781</c:v>
+                  <c:v>0.38188006094507621</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.43034729660938909</c:v>
+                  <c:v>0.45186466143985854</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.50765933578049882</c:v>
+                  <c:v>0.53304230256952378</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.59706513765502311</c:v>
+                  <c:v>0.6269183945377742</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.70014950359276529</c:v>
+                  <c:v>0.73515697877240349</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.81865865558148732</c:v>
+                  <c:v>0.85959158836056171</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.95451064250799922</c:v>
+                  <c:v>1.0022361746333992</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.1098057346592547</c:v>
+                  <c:v>1.1652960213922174</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.286836726490596</c:v>
+                  <c:v>1.3511785628151258</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4880990631216289</c:v>
+                  <c:v>1.5625040162777104</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.7163007021495973</c:v>
+                  <c:v>1.8021157372570771</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.9743716192863507</c:v>
+                  <c:v>2.0730902002506681</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2654728640994213</c:v>
+                  <c:v>2.3787465073043919</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.5930050708304533</c:v>
+                  <c:v>2.722655324371976</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.9606163289232574</c:v>
+                  <c:v>3.10864714536942</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3722093185537796</c:v>
+                  <c:v>3.5408197844814686</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.831947618135997</c:v>
+                  <c:v>4.0235449990427972</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.3442610934874448</c:v>
+                  <c:v>4.5614741481618166</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.9138502820679975</c:v>
+                  <c:v>5.1595427961713973</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.5456896904322104</c:v>
+                  <c:v>5.8229741749538206</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.2450299287233157</c:v>
+                  <c:v>6.5572814251594806</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.0173986126343495</c:v>
+                  <c:v>7.3682685432660664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2927,16 +2674,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3038,15 +2785,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3443,7 +3190,7 @@
   <dimension ref="A2:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,7 +3244,7 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>H4/40</f>
-        <v>0.75</v>
+        <v>0.78749999999999998</v>
       </c>
       <c r="C4">
         <v>5.3579999999999997</v>
@@ -3512,7 +3259,7 @@
         <v>12</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -3568,31 +3315,31 @@
       </c>
       <c r="C8">
         <f>$B$4*EXP($C$4-$D$4*EXP(-1*$E$4*$B8))</f>
-        <v>6.801222499401326E-5</v>
+        <v>7.1412836243713924E-5</v>
       </c>
       <c r="D8">
         <f>$B$4*EXP($C$5-$D$5*EXP(-1*$E$5*$B8))</f>
-        <v>9.7230654201753142E-3</v>
+        <v>1.020921869118408E-2</v>
       </c>
       <c r="E8">
         <f>C8+D8</f>
-        <v>9.7910776451693281E-3</v>
-      </c>
-      <c r="G8">
-        <f>C8*($D$4*$E$4*EXP(-1*$E$4*$A8))</f>
-        <v>5.5424800797046528E-6</v>
-      </c>
-      <c r="H8">
-        <f>D8*($D$4*$E$4*EXP(-1*$E$4*$A8))</f>
-        <v>7.9235602731318462E-4</v>
-      </c>
-      <c r="I8">
-        <f>G8+H8</f>
-        <v>7.9789850739288932E-4</v>
-      </c>
-      <c r="J8">
-        <f>I8/6.25</f>
-        <v>1.2766376118286229E-4</v>
+        <v>1.0280631527427794E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:G47" si="0">C8*($D$4*$E$4*EXP(-1*$E$4*$B8))</f>
+        <v>5.6347469101111042E-6</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ref="H8:H47" si="1">D8*($D$4*$E$4*EXP(-1*$E$4*$B8))</f>
+        <v>8.0554654458023646E-4</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" ref="I8:I47" si="2">G8+H8</f>
+        <v>8.111812914903476E-4</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:J47" si="3">I8/6.25</f>
+        <v>1.2978900663845563E-4</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -3600,36 +3347,36 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B47" si="0">7*A9</f>
+        <f t="shared" ref="B9:B48" si="4">7*A9</f>
         <v>14</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C47" si="1">$B$4*EXP($C$4-$D$4*EXP(-1*$E$4*$B9))</f>
-        <v>1.1694963390665244E-4</v>
+        <f t="shared" ref="C9:C47" si="5">$B$4*EXP($C$4-$D$4*EXP(-1*$E$4*$B9))</f>
+        <v>1.2279711560198505E-4</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D47" si="2">$B$4*EXP($C$5-$D$5*EXP(-1*$E$5*$B9))</f>
-        <v>1.2287663178814686E-2</v>
+        <f t="shared" ref="D9:D47" si="6">$B$4*EXP($C$5-$D$5*EXP(-1*$E$5*$B9))</f>
+        <v>1.2902046337755421E-2</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E47" si="3">C9+D9</f>
-        <v>1.2404612812721339E-2</v>
-      </c>
-      <c r="G9">
-        <f>C9*($D$4*$E$4*EXP(-1*$E$4*$A9))</f>
-        <v>9.4793709894872624E-6</v>
-      </c>
-      <c r="H9">
-        <f>D9*($D$4*$E$4*EXP(-1*$E$4*$A9))</f>
-        <v>9.9597847359504297E-4</v>
-      </c>
-      <c r="I9">
-        <f t="shared" ref="I9:I47" si="4">G9+H9</f>
-        <v>1.0054578445845303E-3</v>
-      </c>
-      <c r="J9">
-        <f t="shared" ref="J9:J47" si="5">I9/6.25</f>
-        <v>1.6087325513352484E-4</v>
+        <f t="shared" ref="E9:E47" si="7">C9+D9</f>
+        <v>1.3024843453357407E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>9.3310553951689572E-6</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="1"/>
+        <v>9.8039525194422786E-4</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="2"/>
+        <v>9.8972630733939679E-4</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5835620917430349E-4</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -3637,36 +3384,36 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>1.9711061015858003E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.0696614066650904E-4</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
-        <v>1.5462788886750765E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.6235928331088303E-2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
-        <v>1.5659899496909345E-2</v>
-      </c>
-      <c r="G10">
-        <f>C10*($D$4*$E$4*EXP(-1*$E$4*$A10))</f>
-        <v>1.5891106992681293E-5</v>
-      </c>
-      <c r="H10">
-        <f>D10*($D$4*$E$4*EXP(-1*$E$4*$A10))</f>
-        <v>1.2466139311674374E-3</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>1.2625050381601186E-3</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="5"/>
-        <v>2.0200080610561897E-4</v>
+        <f t="shared" si="7"/>
+        <v>1.6442894471754812E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>1.514559617661504E-5</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>1.188130644284263E-3</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2032762404608781E-3</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="3"/>
+        <v>1.925241984737405E-4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -3674,36 +3421,36 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
-        <v>3.2586818873865859E-4</v>
+        <f t="shared" si="5"/>
+        <v>3.4216159817559153E-4</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
-        <v>1.9377260065973095E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.0346123069271749E-2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
-        <v>1.9703128254711755E-2</v>
-      </c>
-      <c r="G11">
-        <f>C11*($D$4*$E$4*EXP(-1*$E$4*$A11))</f>
-        <v>2.6130613829907702E-5</v>
-      </c>
-      <c r="H11">
-        <f>D11*($D$4*$E$4*EXP(-1*$E$4*$A11))</f>
-        <v>1.5538175169093036E-3</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>1.5799481307392114E-3</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>2.5279170091827382E-4</v>
+        <f t="shared" si="7"/>
+        <v>2.0688284667447342E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.4113641912570266E-5</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4338813257171153E-3</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4579949676296856E-3</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="3"/>
+        <v>2.332791948207497E-4</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -3711,36 +3458,36 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>5.2881583501794484E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.5525662676884208E-4</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
-        <v>2.4183318083505614E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.5392483987680896E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
-        <v>2.471213391852356E-2</v>
-      </c>
-      <c r="G12">
-        <f>C12*($D$4*$E$4*EXP(-1*$E$4*$A12))</f>
-        <v>4.2176990914111152E-5</v>
-      </c>
-      <c r="H12">
-        <f>D12*($D$4*$E$4*EXP(-1*$E$4*$A12))</f>
-        <v>1.9287992520996731E-3</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
-        <v>1.9709762430137842E-3</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>3.1535619888220544E-4</v>
+        <f t="shared" si="7"/>
+        <v>2.5947740614449738E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>3.7685107787432621E-5</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7233805954463368E-3</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.7610657032337694E-3</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="3"/>
+        <v>2.8177051251740312E-4</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -3748,36 +3495,36 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
-        <v>8.4293813413467136E-4</v>
+        <f t="shared" si="5"/>
+        <v>8.8508504084140499E-4</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
-        <v>3.0060122989741526E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.1563129139228603E-2</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
-        <v>3.0903061123876197E-2</v>
-      </c>
-      <c r="G13">
-        <f>C13*($D$4*$E$4*EXP(-1*$E$4*$A13))</f>
-        <v>6.6869848309820785E-5</v>
-      </c>
-      <c r="H13">
-        <f>D13*($D$4*$E$4*EXP(-1*$E$4*$A13))</f>
-        <v>2.384654084444859E-3</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="4"/>
-        <v>2.4515239327546796E-3</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>3.9224382924074873E-4</v>
+        <f t="shared" si="7"/>
+        <v>3.2448214180070011E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>5.7850282202192031E-5</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="1"/>
+        <v>2.0630062012490704E-3</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="2"/>
+        <v>2.1208564834512625E-3</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="3"/>
+        <v>3.39337037352202E-4</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -3785,36 +3532,36 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
-        <v>1.3206962350561075E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.3867310468089129E-3</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
-        <v>3.7217632310038634E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.9078513925540563E-2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
-        <v>3.8538328545094744E-2</v>
-      </c>
-      <c r="G14">
-        <f>C14*($D$4*$E$4*EXP(-1*$E$4*$A14))</f>
-        <v>1.0420800266608693E-4</v>
-      </c>
-      <c r="H14">
-        <f>D14*($D$4*$E$4*EXP(-1*$E$4*$A14))</f>
-        <v>2.9366140555592505E-3</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="4"/>
-        <v>3.0408220582253376E-3</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>4.8653152931605399E-4</v>
+        <f t="shared" si="7"/>
+        <v>4.0465244972349476E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>8.728853203987221E-5</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4598180899675056E-3</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5471066220073778E-3</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="3"/>
+        <v>4.0753705952118044E-4</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -3822,36 +3569,36 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
-        <v>2.035179749598973E-3</v>
+        <f t="shared" si="5"/>
+        <v>2.1369387370789215E-3</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
-        <v>4.5900884270609579E-2</v>
+        <f t="shared" si="6"/>
+        <v>4.8195928484140053E-2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
-        <v>4.7936064020208551E-2</v>
-      </c>
-      <c r="G15">
-        <f>C15*($D$4*$E$4*EXP(-1*$E$4*$A15))</f>
-        <v>1.5972187526488432E-4</v>
-      </c>
-      <c r="H15">
-        <f>D15*($D$4*$E$4*EXP(-1*$E$4*$A15))</f>
-        <v>3.602323241208951E-3</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="4"/>
-        <v>3.7620451164738352E-3</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>6.0192721863581359E-4</v>
+        <f t="shared" si="7"/>
+        <v>5.0332867221218977E-2</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2953928409825501E-4</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="1"/>
+        <v>2.9215933821389768E-3</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0511326662372319E-3</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="3"/>
+        <v>4.8818122659795711E-4</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3859,36 +3606,36 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>3.0864666142974592E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.2407899450123323E-3</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
-        <v>5.6394703854019748E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.9214439046720739E-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
-        <v>5.9481170468317204E-2</v>
-      </c>
-      <c r="G16">
-        <f>C16*($D$4*$E$4*EXP(-1*$E$4*$A16))</f>
-        <v>2.40927684741692E-4</v>
-      </c>
-      <c r="H16">
-        <f>D16*($D$4*$E$4*EXP(-1*$E$4*$A16))</f>
-        <v>4.4021358819509001E-3</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="4"/>
-        <v>4.6430635666925924E-3</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>7.4289017067081479E-4</v>
+        <f t="shared" si="7"/>
+        <v>6.2455228991733072E-2</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8919287348140434E-4</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="1"/>
+        <v>3.4568577615097279E-3</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="2"/>
+        <v>3.6460506349911322E-3</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="3"/>
+        <v>5.8336810159858113E-4</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3896,36 +3643,36 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
-        <v>4.6093099255578628E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.8397754218357557E-3</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
-        <v>6.9028847475679306E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.2480289849463267E-2</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
-        <v>7.3638157401237164E-2</v>
-      </c>
-      <c r="G17">
-        <f>C17*($D$4*$E$4*EXP(-1*$E$4*$A17))</f>
-        <v>3.5786937090685604E-4</v>
-      </c>
-      <c r="H17">
-        <f>D17*($D$4*$E$4*EXP(-1*$E$4*$A17))</f>
-        <v>5.3594378810526266E-3</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="4"/>
-        <v>5.7173072519594824E-3</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="5"/>
-        <v>9.1476916031351719E-4</v>
+        <f t="shared" si="7"/>
+        <v>7.7320065271299018E-2</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7209688514189396E-4</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="1"/>
+        <v>4.0749124459870181E-3</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="2"/>
+        <v>4.3470093311289123E-3</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="3"/>
+        <v>6.9552149298062599E-4</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3933,36 +3680,36 @@
         <v>11</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
-        <v>6.7822346306760008E-3</v>
+        <f t="shared" si="5"/>
+        <v>7.121346362209801E-3</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
-        <v>8.4183598939493787E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.8392778886468473E-2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
-        <v>9.0965833570169782E-2</v>
-      </c>
-      <c r="G18">
-        <f>C18*($D$4*$E$4*EXP(-1*$E$4*$A18))</f>
-        <v>5.2375107211785784E-4</v>
-      </c>
-      <c r="H18">
-        <f>D18*($D$4*$E$4*EXP(-1*$E$4*$A18))</f>
-        <v>6.5009915758259384E-3</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="4"/>
-        <v>7.0247426479437963E-3</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="5"/>
-        <v>1.1239588236710075E-3</v>
+        <f t="shared" si="7"/>
+        <v>9.5514125248678278E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8557151279722712E-4</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="1"/>
+        <v>4.785855896079552E-3</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="2"/>
+        <v>5.1714274088767789E-3</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="3"/>
+        <v>8.2742838542028462E-4</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3970,36 +3717,36 @@
         <v>12</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
-        <v>9.8380767700469163E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.0329980608549262E-2</v>
       </c>
       <c r="D19">
-        <f t="shared" si="2"/>
-        <v>0.10229582566649324</v>
+        <f t="shared" si="6"/>
+        <v>0.10741061694981791</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
-        <v>0.11213390243654016</v>
-      </c>
-      <c r="G19">
-        <f>C19*($D$4*$E$4*EXP(-1*$E$4*$A19))</f>
-        <v>7.5565892789874046E-4</v>
-      </c>
-      <c r="H19">
-        <f>D19*($D$4*$E$4*EXP(-1*$E$4*$A19))</f>
-        <v>7.8573033895211319E-3</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="4"/>
-        <v>8.6129623174198717E-3</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
-        <v>1.3780739707871794E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.11774059755836716</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3862537113401538E-4</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="1"/>
+        <v>5.6005994213046478E-3</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="2"/>
+        <v>6.1392247924386628E-3</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="3"/>
+        <v>9.82275966790186E-4</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -4007,36 +3754,36 @@
         <v>13</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
-        <v>1.4075934382809088E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.4779731101949542E-2</v>
       </c>
       <c r="D20">
-        <f t="shared" si="2"/>
-        <v>0.12386550000295146</v>
+        <f t="shared" si="6"/>
+        <v>0.13005877500309904</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
-        <v>0.13794143438576056</v>
-      </c>
-      <c r="G20">
-        <f>C20*($D$4*$E$4*EXP(-1*$E$4*$A20))</f>
-        <v>1.0753660958394081E-3</v>
-      </c>
-      <c r="H20">
-        <f>D20*($D$4*$E$4*EXP(-1*$E$4*$A20))</f>
-        <v>9.4630136461880589E-3</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="4"/>
-        <v>1.0538379742027468E-2</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="5"/>
-        <v>1.6861407587243948E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.14483850610504859</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="0"/>
+        <v>7.421612970592873E-4</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5308758653606211E-3</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="2"/>
+        <v>7.2730371624199087E-3</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1636859459871853E-3</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -4044,36 +3791,36 @@
         <v>14</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
-        <v>1.9874424073124966E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.0868145276781214E-2</v>
       </c>
       <c r="D21">
-        <f t="shared" si="2"/>
-        <v>0.14946268572300453</v>
+        <f t="shared" si="6"/>
+        <v>0.15693582000915474</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
-        <v>0.16933710979612948</v>
-      </c>
-      <c r="G21">
-        <f>C21*($D$4*$E$4*EXP(-1*$E$4*$A21))</f>
-        <v>1.5102093486828666E-3</v>
-      </c>
-      <c r="H21">
-        <f>D21*($D$4*$E$4*EXP(-1*$E$4*$A21))</f>
-        <v>1.1357307483609483E-2</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="4"/>
-        <v>1.2867516832292349E-2</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="5"/>
-        <v>2.0588026931667759E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.17780396528593595</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0091601465842578E-3</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="1"/>
+        <v>7.5892405877091649E-3</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="2"/>
+        <v>8.598400734293422E-3</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3757441174869476E-3</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -4081,36 +3828,36 @@
         <v>15</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
-        <v>2.7706053649323156E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.9091356331789314E-2</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
-        <v>0.17973498467474197</v>
+        <f t="shared" si="6"/>
+        <v>0.18872173390847907</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
-        <v>0.20744103832406513</v>
-      </c>
-      <c r="G22">
-        <f>C22*($D$4*$E$4*EXP(-1*$E$4*$A22))</f>
-        <v>2.0940197260457677E-3</v>
-      </c>
-      <c r="H22">
-        <f>D22*($D$4*$E$4*EXP(-1*$E$4*$A22))</f>
-        <v>1.3584345433426169E-2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="4"/>
-        <v>1.5678365159471935E-2</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="5"/>
-        <v>2.5085384255155098E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.21781309024026838</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3548296093178387E-3</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="1"/>
+        <v>8.789064012859775E-3</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0143893622177614E-2</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6230229795484183E-3</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -4118,36 +3865,36 @@
         <v>16</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>3.8152433331449742E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.0060054998022232E-2</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
-        <v>0.21541543291884618</v>
+        <f t="shared" si="6"/>
+        <v>0.22618620456478847</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
-        <v>0.25356786625029593</v>
-      </c>
-      <c r="G23">
-        <f>C23*($D$4*$E$4*EXP(-1*$E$4*$A23))</f>
-        <v>2.8680837935215618E-3</v>
-      </c>
-      <c r="H23">
-        <f>D23*($D$4*$E$4*EXP(-1*$E$4*$A23))</f>
-        <v>1.6193711857421314E-2</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="4"/>
-        <v>1.9061795650942875E-2</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="5"/>
-        <v>3.0498873041508601E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.26624625956281067</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7967047688661655E-3</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0144515088992188E-2</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1941219857858353E-2</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="3"/>
+        <v>1.9105951772573366E-3</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4155,36 +3902,36 @@
         <v>17</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>119</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
-        <v>5.1919960751586745E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.4515958789166083E-2</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
-        <v>0.25733082972662075</v>
+        <f t="shared" si="6"/>
+        <v>0.27019737121295179</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
-        <v>0.30925079047820747</v>
-      </c>
-      <c r="G24">
-        <f>C24*($D$4*$E$4*EXP(-1*$E$4*$A24))</f>
-        <v>3.8821064915905063E-3</v>
-      </c>
-      <c r="H24">
-        <f>D24*($D$4*$E$4*EXP(-1*$E$4*$A24))</f>
-        <v>1.9240879039716056E-2</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="4"/>
-        <v>2.3122985531306563E-2</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="5"/>
-        <v>3.6996776850090501E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.32471333000211788</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3546876375447178E-3</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1670535084098276E-2</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4025222721642994E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2440356354628791E-3</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -4192,36 +3939,36 @@
         <v>18</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>6.9855533827244479E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.3348310518606699E-2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
-        <v>0.3064104765016652</v>
+        <f t="shared" si="6"/>
+        <v>0.3217310003267484</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
-        <v>0.37626601032890966</v>
-      </c>
-      <c r="G25">
-        <f>C25*($D$4*$E$4*EXP(-1*$E$4*$A25))</f>
-        <v>5.19514173460603E-3</v>
-      </c>
-      <c r="H25">
-        <f>D25*($D$4*$E$4*EXP(-1*$E$4*$A25))</f>
-        <v>2.2787684341959498E-2</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="4"/>
-        <v>2.7982826076565527E-2</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="5"/>
-        <v>4.477252172250484E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.39507931084535508</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="0"/>
+        <v>3.0510142344812451E-3</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3382801249686448E-2</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6433815484167693E-2</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="3"/>
+        <v>2.6294104774668308E-3</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -4229,36 +3976,36 @@
         <v>19</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>9.2961776155498846E-2</v>
+        <f t="shared" si="5"/>
+        <v>9.7609864963273785E-2</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
-        <v>0.36369529613816781</v>
+        <f t="shared" si="6"/>
+        <v>0.38188006094507621</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
-        <v>0.45665707229366664</v>
-      </c>
-      <c r="G26">
-        <f>C26*($D$4*$E$4*EXP(-1*$E$4*$A26))</f>
-        <v>6.876453226712871E-3</v>
-      </c>
-      <c r="H26">
-        <f>D26*($D$4*$E$4*EXP(-1*$E$4*$A26))</f>
-        <v>2.6902817438494722E-2</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="4"/>
-        <v>3.3779270665207591E-2</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="5"/>
-        <v>5.4046833064332143E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.47948992590834999</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="0"/>
+        <v>3.910139940694478E-3</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" si="1"/>
+        <v>1.5297679998000302E-2</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="2"/>
+        <v>1.9207819938694779E-2</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="3"/>
+        <v>3.0732511901911648E-3</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -4266,36 +4013,36 @@
         <v>20</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
-        <v>0.12241120710999331</v>
+        <f t="shared" si="5"/>
+        <v>0.12853176746549297</v>
       </c>
       <c r="D27">
-        <f t="shared" si="2"/>
-        <v>0.43034729660938909</v>
+        <f t="shared" si="6"/>
+        <v>0.45186466143985854</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
-        <v>0.5527585037193824</v>
-      </c>
-      <c r="G27">
-        <f>C27*($D$4*$E$4*EXP(-1*$E$4*$A27))</f>
-        <v>9.0062657297743879E-3</v>
-      </c>
-      <c r="H27">
-        <f>D27*($D$4*$E$4*EXP(-1*$E$4*$A27))</f>
-        <v>3.166231426728397E-2</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="4"/>
-        <v>4.0668579997058356E-2</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="5"/>
-        <v>6.5069727995293366E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.58039642890535148</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="0"/>
+        <v>4.958536771526397E-3</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" si="1"/>
+        <v>1.743216936703525E-2</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2390706138561648E-2</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="3"/>
+        <v>3.5825129821698636E-3</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -4303,36 +4050,36 @@
         <v>21</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>147</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>0.1595587578323498</v>
+        <f t="shared" si="5"/>
+        <v>0.16753669572396726</v>
       </c>
       <c r="D28">
-        <f t="shared" si="2"/>
-        <v>0.50765933578049882</v>
+        <f t="shared" si="6"/>
+        <v>0.53304230256952378</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
-        <v>0.66721809361284867</v>
-      </c>
-      <c r="G28">
-        <f>C28*($D$4*$E$4*EXP(-1*$E$4*$A28))</f>
-        <v>1.1676366505113727E-2</v>
-      </c>
-      <c r="H28">
-        <f>D28*($D$4*$E$4*EXP(-1*$E$4*$A28))</f>
-        <v>3.715005396660153E-2</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="4"/>
-        <v>4.8826420471715259E-2</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="5"/>
-        <v>7.8122272754744416E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.70057899829349102</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="0"/>
+        <v>6.2243997144107348E-3</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="1"/>
+        <v>1.9803830686437138E-2</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="2"/>
+        <v>2.6028230400847872E-2</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="3"/>
+        <v>4.1645168641356598E-3</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -4340,36 +4087,36 @@
         <v>22</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>154</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
-        <v>0.20595202818678859</v>
+        <f t="shared" si="5"/>
+        <v>0.21624962959612803</v>
       </c>
       <c r="D29">
-        <f t="shared" si="2"/>
-        <v>0.59706513765502311</v>
+        <f t="shared" si="6"/>
+        <v>0.6269183945377742</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
-        <v>0.80301716584181171</v>
-      </c>
-      <c r="G29">
-        <f>C29*($D$4*$E$4*EXP(-1*$E$4*$A29))</f>
-        <v>1.4990518014444293E-2</v>
-      </c>
-      <c r="H29">
-        <f>D29*($D$4*$E$4*EXP(-1*$E$4*$A29))</f>
-        <v>4.3458254723749451E-2</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="4"/>
-        <v>5.8448772738193745E-2</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="5"/>
-        <v>9.3518036381109986E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.84316802413390224</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>7.7372631975185305E-3</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2430709504398492E-2</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0167972701917022E-2</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="3"/>
+        <v>4.8268756323067239E-3</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -4377,36 +4124,36 @@
         <v>23</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>161</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>0.26333870048840585</v>
+        <f t="shared" si="5"/>
+        <v>0.27650563551282614</v>
       </c>
       <c r="D30">
-        <f t="shared" si="2"/>
-        <v>0.70014950359276529</v>
+        <f t="shared" si="6"/>
+        <v>0.73515697877240349</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
-        <v>0.9634882040811712</v>
-      </c>
-      <c r="G30">
-        <f>C30*($D$4*$E$4*EXP(-1*$E$4*$A30))</f>
-        <v>1.906464625103213E-2</v>
-      </c>
-      <c r="H30">
-        <f>D30*($D$4*$E$4*EXP(-1*$E$4*$A30))</f>
-        <v>5.068796414684025E-2</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="4"/>
-        <v>6.975261039787238E-2</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="5"/>
-        <v>1.1160417663659581E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.0116626142852296</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5275328570834424E-3</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5331245988450629E-2</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4858778845534073E-2</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="3"/>
+        <v>5.5774046152854521E-3</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -4414,36 +4161,36 @@
         <v>24</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>0.3336705738508271</v>
+        <f t="shared" si="5"/>
+        <v>0.35035410254336841</v>
       </c>
       <c r="D31">
-        <f t="shared" si="2"/>
-        <v>0.81865865558148732</v>
+        <f t="shared" si="6"/>
+        <v>0.85959158836056171</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
-        <v>1.1523292294323144</v>
-      </c>
-      <c r="G31">
-        <f>C31*($D$4*$E$4*EXP(-1*$E$4*$A31))</f>
-        <v>2.4026774206671184E-2</v>
-      </c>
-      <c r="H31">
-        <f>D31*($D$4*$E$4*EXP(-1*$E$4*$A31))</f>
-        <v>5.8949539490368907E-2</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="4"/>
-        <v>8.2976313697040088E-2</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="5"/>
-        <v>1.3276210191526415E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.2099456909039301</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1625941816347123E-2</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="1"/>
+        <v>2.8524175168932835E-2</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0150116985279954E-2</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="3"/>
+        <v>6.4240187176447926E-3</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -4451,591 +4198,617 @@
         <v>25</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>175</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>0.4191037571419699</v>
+        <f t="shared" si="5"/>
+        <v>0.44005894499906839</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
-        <v>0.95451064250799922</v>
+        <f t="shared" si="6"/>
+        <v>1.0022361746333992</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
-        <v>1.373614399649969</v>
-      </c>
-      <c r="G32">
-        <f>C32*($D$4*$E$4*EXP(-1*$E$4*$A32))</f>
-        <v>3.0016676775815605E-2</v>
-      </c>
-      <c r="H32">
-        <f>D32*($D$4*$E$4*EXP(-1*$E$4*$A32))</f>
-        <v>6.8363112825860897E-2</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="4"/>
-        <v>9.8379789601676509E-2</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="5"/>
-        <v>1.5740766336268242E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>1.4422951196324676</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4062944437473085E-2</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="1"/>
+        <v>3.2028417550119113E-2</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="2"/>
+        <v>4.60913619875922E-2</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="3"/>
+        <v>7.3746179180147519E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>26</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>182</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>0.52199465606193418</v>
+        <f t="shared" si="5"/>
+        <v>0.54809438886503081</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
-        <v>1.1098057346592547</v>
+        <f t="shared" si="6"/>
+        <v>1.1652960213922174</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
-        <v>1.6318003907211889</v>
-      </c>
-      <c r="G33">
-        <f>C33*($D$4*$E$4*EXP(-1*$E$4*$A33))</f>
-        <v>3.7185241565954381E-2</v>
-      </c>
-      <c r="H33">
-        <f>D33*($D$4*$E$4*EXP(-1*$E$4*$A33))</f>
-        <v>7.9059036055896717E-2</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="4"/>
-        <v>0.11624427762185111</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="5"/>
-        <v>1.8599084419496176E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>1.7133904102572481</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="0"/>
+        <v>1.686806374002852E-2</v>
+      </c>
+      <c r="H33" s="3">
+        <f t="shared" si="1"/>
+        <v>3.5862960767667991E-2</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="2"/>
+        <v>5.2731024507696511E-2</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="3"/>
+        <v>8.4369639212314423E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>27</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>189</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
-        <v>0.64489150668751249</v>
+        <f t="shared" si="5"/>
+        <v>0.67713608202188813</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
-        <v>1.286836726490596</v>
+        <f t="shared" si="6"/>
+        <v>1.3511785628151258</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
-        <v>1.9317282331781085</v>
-      </c>
-      <c r="G34">
-        <f>C34*($D$4*$E$4*EXP(-1*$E$4*$A34))</f>
-        <v>4.569352925233789E-2</v>
-      </c>
-      <c r="H34">
-        <f>D34*($D$4*$E$4*EXP(-1*$E$4*$A34))</f>
-        <v>9.1178300528266781E-2</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="4"/>
-        <v>0.13687182978060466</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="5"/>
-        <v>2.1899492764896746E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.028314644837014</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0069211211991858E-2</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="1"/>
+        <v>4.0046733119408373E-2</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="2"/>
+        <v>6.0115944331400231E-2</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="3"/>
+        <v>9.6185510930240376E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>28</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>196</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
-        <v>0.79052133881471387</v>
+        <f t="shared" si="5"/>
+        <v>0.83004740575544955</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
-        <v>1.4880990631216289</v>
+        <f t="shared" si="6"/>
+        <v>1.5625040162777104</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
-        <v>2.278620401936343</v>
-      </c>
-      <c r="G35">
-        <f>C35*($D$4*$E$4*EXP(-1*$E$4*$A35))</f>
-        <v>5.5711536858794923E-2</v>
-      </c>
-      <c r="H35">
-        <f>D35*($D$4*$E$4*EXP(-1*$E$4*$A35))</f>
-        <v>0.10487292592119429</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="4"/>
-        <v>0.16058446277998922</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="5"/>
-        <v>2.5693514044798277E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.3925514220331601</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3691999435515018E-2</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="1"/>
+        <v>4.459846993672556E-2</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="2"/>
+        <v>6.8290469372240578E-2</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0926475099558493E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>29</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>203</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
-        <v>0.96177239169730955</v>
+        <f t="shared" si="5"/>
+        <v>1.0098610112821749</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
-        <v>1.7163007021495973</v>
+        <f t="shared" si="6"/>
+        <v>1.8021157372570771</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
-        <v>2.6780730938469066</v>
-      </c>
-      <c r="G36">
-        <f>C36*($D$4*$E$4*EXP(-1*$E$4*$A36))</f>
-        <v>6.7416677210304088E-2</v>
-      </c>
-      <c r="H36">
-        <f>D36*($D$4*$E$4*EXP(-1*$E$4*$A36))</f>
-        <v>0.12030631304402552</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="4"/>
-        <v>0.18772299025432959</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="5"/>
-        <v>3.0035678440692735E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.8119767485392519</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7759068728593857E-2</v>
+      </c>
+      <c r="H36" s="3">
+        <f t="shared" si="1"/>
+        <v>4.9536573893357111E-2</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="2"/>
+        <v>7.7295642621950961E-2</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="3"/>
+        <v>1.2367302819512154E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>30</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>1.1616721460996831</v>
+        <f t="shared" si="5"/>
+        <v>1.2197557534046672</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
-        <v>1.9743716192863507</v>
+        <f t="shared" si="6"/>
+        <v>2.0730902002506681</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
-        <v>3.1360437653860336</v>
-      </c>
-      <c r="G37">
-        <f>C37*($D$4*$E$4*EXP(-1*$E$4*$A37))</f>
-        <v>8.0991997334215055E-2</v>
-      </c>
-      <c r="H37">
-        <f>D37*($D$4*$E$4*EXP(-1*$E$4*$A37))</f>
-        <v>0.13765355523318903</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="4"/>
-        <v>0.21864555256740409</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="5"/>
-        <v>3.4983288410784658E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>3.2928459536553354</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2289448841778895E-2</v>
+      </c>
+      <c r="H37" s="3">
+        <f t="shared" si="1"/>
+        <v>5.4878970464818454E-2</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="2"/>
+        <v>8.7168419306597356E-2</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3946947089055577E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>31</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>217</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>1.3933612737606456</v>
+        <f t="shared" si="5"/>
+        <v>1.4630293374486778</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
-        <v>2.2654728640994213</v>
+        <f t="shared" si="6"/>
+        <v>2.3787465073043919</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
-        <v>3.6588341378600671</v>
-      </c>
-      <c r="G38">
-        <f>C38*($D$4*$E$4*EXP(-1*$E$4*$A38))</f>
-        <v>9.6624167360977328E-2</v>
-      </c>
-      <c r="H38">
-        <f>D38*($D$4*$E$4*EXP(-1*$E$4*$A38))</f>
-        <v>0.15710170312232902</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="4"/>
-        <v>0.25372587048330636</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="5"/>
-        <v>4.0596139277329017E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>3.8417758447530694</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="0"/>
+        <v>3.7297975678324685E-2</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="1"/>
+        <v>6.0642959852779663E-2</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="2"/>
+        <v>9.7940935531104348E-2</v>
+      </c>
+      <c r="J38" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5670549684976696E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>32</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>224</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
-        <v>1.6600639325924096</v>
+        <f t="shared" si="5"/>
+        <v>1.7430671292220299</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
-        <v>2.5930050708304533</v>
+        <f t="shared" si="6"/>
+        <v>2.722655324371976</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
-        <v>4.2530690034228629</v>
-      </c>
-      <c r="G39">
-        <f>C39*($D$4*$E$4*EXP(-1*$E$4*$A39))</f>
-        <v>0.11450127911935272</v>
-      </c>
-      <c r="H39">
-        <f>D39*($D$4*$E$4*EXP(-1*$E$4*$A39))</f>
-        <v>0.1788499777291121</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="4"/>
-        <v>0.2933512568484648</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="5"/>
-        <v>4.6936201095754367E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>4.4657224535940063</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2794781109091004E-2</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="1"/>
+        <v>6.6845066772616701E-2</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="2"/>
+        <v>0.10963984788170771</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="3"/>
+        <v>1.7542375661073233E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>33</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>231</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
-        <v>1.9650549480984005</v>
+        <f t="shared" si="5"/>
+        <v>2.0633076955033203</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
-        <v>2.9606163289232574</v>
+        <f t="shared" si="6"/>
+        <v>3.10864714536942</v>
       </c>
       <c r="E40">
-        <f t="shared" si="3"/>
-        <v>4.9256712770216584</v>
-      </c>
-      <c r="G40">
-        <f>C40*($D$4*$E$4*EXP(-1*$E$4*$A40))</f>
-        <v>0.13481049983318452</v>
-      </c>
-      <c r="H40">
-        <f>D40*($D$4*$E$4*EXP(-1*$E$4*$A40))</f>
-        <v>0.203109927029097</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="4"/>
-        <v>0.33792042686228152</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="5"/>
-        <v>5.4067268297965043E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>5.1719548408727398</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8784871353728304E-2</v>
+      </c>
+      <c r="H40" s="3">
+        <f t="shared" si="1"/>
+        <v>7.3500889567509414E-2</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="2"/>
+        <v>0.12228576092123772</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="3"/>
+        <v>1.9565721747398034E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>34</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>238</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
-        <v>2.3116245144007945</v>
+        <f t="shared" si="5"/>
+        <v>2.4272057401208342</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
-        <v>3.3722093185537796</v>
+        <f t="shared" si="6"/>
+        <v>3.5408197844814686</v>
       </c>
       <c r="E41">
-        <f t="shared" si="3"/>
-        <v>5.6838338329545746</v>
-      </c>
-      <c r="G41">
-        <f>C41*($D$4*$E$4*EXP(-1*$E$4*$A41))</f>
-        <v>0.15773563088775461</v>
-      </c>
-      <c r="H41">
-        <f>D41*($D$4*$E$4*EXP(-1*$E$4*$A41))</f>
-        <v>0.23010552147805285</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="4"/>
-        <v>0.38784115236580746</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="5"/>
-        <v>6.2054584378529197E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>5.9680255246023028</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="0"/>
+        <v>5.5267806251335858E-2</v>
+      </c>
+      <c r="H41" s="3">
+        <f t="shared" si="1"/>
+        <v>8.0624950157655917E-2</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="2"/>
+        <v>0.13589275640899179</v>
+      </c>
+      <c r="J41" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1742841025438685E-2</v>
+      </c>
+      <c r="K41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>35</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>245</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
-        <v>2.703041118834955</v>
+        <f t="shared" si="5"/>
+        <v>2.8381931747767029</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
-        <v>3.831947618135997</v>
+        <f t="shared" si="6"/>
+        <v>4.0235449990427972</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
-        <v>6.5349887369709521</v>
-      </c>
-      <c r="G42">
-        <f>C42*($D$4*$E$4*EXP(-1*$E$4*$A42))</f>
-        <v>0.18345462441381136</v>
-      </c>
-      <c r="H42">
-        <f>D42*($D$4*$E$4*EXP(-1*$E$4*$A42))</f>
-        <v>0.26007318429604032</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="4"/>
-        <v>0.44352780870985165</v>
-      </c>
-      <c r="J42">
+        <f t="shared" si="7"/>
+        <v>6.8617381738195</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="0"/>
+        <v>6.2237488219597688E-2</v>
+      </c>
+      <c r="H42" s="3">
+        <f t="shared" si="1"/>
+        <v>8.8230546357595585E-2</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="2"/>
+        <v>0.15046803457719327</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4074885532350921E-2</v>
+      </c>
+      <c r="K42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>36</v>
+      </c>
+      <c r="B43" s="2">
+        <f t="shared" si="4"/>
+        <v>252</v>
+      </c>
+      <c r="C43" s="2">
         <f t="shared" si="5"/>
-        <v>7.0964449393576268E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>36</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>252</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="1"/>
-        <v>3.1425134403857591</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="2"/>
-        <v>4.3442610934874448</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="3"/>
-        <v>7.4867745338732039</v>
-      </c>
-      <c r="G43">
-        <f>C43*($D$4*$E$4*EXP(-1*$E$4*$A43))</f>
-        <v>0.21213711139656924</v>
-      </c>
-      <c r="H43">
-        <f>D43*($D$4*$E$4*EXP(-1*$E$4*$A43))</f>
-        <v>0.29326175273630634</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="4"/>
-        <v>0.5053988641328756</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="5"/>
-        <v>8.0863818261260101E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.299639112405047</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="6"/>
+        <v>4.5614741481618166</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="7"/>
+        <v>7.8611132605668637</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3">
+        <f>C43*($D$4*$E$4*EXP(-1*$E$4*$B43))</f>
+        <v>6.9682065980887012E-2</v>
+      </c>
+      <c r="H43" s="3">
+        <f>D43*($D$4*$E$4*EXP(-1*$E$4*$B43))</f>
+        <v>9.632960809785189E-2</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" ref="I9:I47" si="8">G43+H43</f>
+        <v>0.1660116740787389</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" ref="J9:J47" si="9">I43/6.25</f>
+        <v>2.6561867852598224E-2</v>
+      </c>
+      <c r="K43" s="2">
+        <v>5</v>
+      </c>
+      <c r="M43">
+        <f>EXP(-1*$E$4*$A43)</f>
+        <v>0.82392151697372606</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>37</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>259</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
-        <v>3.6331519935904493</v>
+        <f t="shared" si="5"/>
+        <v>3.8148095932699717</v>
       </c>
       <c r="D44">
-        <f t="shared" si="2"/>
-        <v>4.9138502820679975</v>
+        <f t="shared" si="6"/>
+        <v>5.1595427961713973</v>
       </c>
       <c r="E44">
-        <f t="shared" si="3"/>
-        <v>8.5470022756584463</v>
-      </c>
-      <c r="G44">
-        <f>C44*($D$4*$E$4*EXP(-1*$E$4*$A44))</f>
-        <v>0.24394199420023857</v>
-      </c>
-      <c r="H44">
-        <f>D44*($D$4*$E$4*EXP(-1*$E$4*$A44))</f>
-        <v>0.32993236702559936</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="4"/>
-        <v>0.5738743612258379</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="5"/>
-        <v>9.1819897796134059E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>8.9743523894413695</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" ref="G44:G47" si="10">C44*($D$4*$E$4*EXP(-1*$E$4*$B44))</f>
+        <v>7.7583954392270393E-2</v>
+      </c>
+      <c r="H44" s="3">
+        <f t="shared" ref="H44:H47" si="11">D44*($D$4*$E$4*EXP(-1*$E$4*$B44))</f>
+        <v>0.10493255906908906</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" ref="I44:I47" si="12">G44+H44</f>
+        <v>0.18251651346135944</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" ref="J44:J47" si="13">I44/6.25</f>
+        <v>2.9202642153817512E-2</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>38</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>266</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
-        <v>4.1779312863227629</v>
+        <f t="shared" si="5"/>
+        <v>4.3868278506389009</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
-        <v>5.5456896904322104</v>
+        <f t="shared" si="6"/>
+        <v>5.8229741749538206</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
-        <v>9.7236209767549724</v>
-      </c>
-      <c r="G45">
-        <f>C45*($D$4*$E$4*EXP(-1*$E$4*$A45))</f>
-        <v>0.27901515392631904</v>
-      </c>
-      <c r="H45">
-        <f>D45*($D$4*$E$4*EXP(-1*$E$4*$A45))</f>
-        <v>0.37035828417499872</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="4"/>
-        <v>0.64937343810131776</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="5"/>
-        <v>0.10389975009621084</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>10.209802025592722</v>
+      </c>
+      <c r="G45" s="3">
+        <f t="shared" si="10"/>
+        <v>8.591996811537965E-2</v>
+      </c>
+      <c r="H45" s="3">
+        <f t="shared" si="11"/>
+        <v>0.11404818526805102</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="12"/>
+        <v>0.19996815338343066</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="13"/>
+        <v>3.1994904541348908E-2</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>39</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>273</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
-        <v>4.7796532335225521</v>
+        <f t="shared" si="5"/>
+        <v>5.0186358951986803</v>
       </c>
       <c r="D46">
-        <f t="shared" si="2"/>
-        <v>6.2450299287233157</v>
+        <f t="shared" si="6"/>
+        <v>6.5572814251594806</v>
       </c>
       <c r="E46">
-        <f t="shared" si="3"/>
-        <v>11.024683162245868</v>
-      </c>
-      <c r="G46">
-        <f>C46*($D$4*$E$4*EXP(-1*$E$4*$A46))</f>
-        <v>0.31748731907913974</v>
-      </c>
-      <c r="H46">
-        <f>D46*($D$4*$E$4*EXP(-1*$E$4*$A46))</f>
-        <v>0.41482461441624607</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="4"/>
-        <v>0.73231193349538581</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="5"/>
-        <v>0.11716990935926173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>11.575917320358162</v>
+      </c>
+      <c r="G46" s="3">
+        <f t="shared" si="10"/>
+        <v>9.4661563542256924E-2</v>
+      </c>
+      <c r="H46" s="3">
+        <f t="shared" si="11"/>
+        <v>0.12368351186545318</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" si="12"/>
+        <v>0.21834507540771009</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="13"/>
+        <v>3.4935212065233617E-2</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>40</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
-        <v>5.440912521714206</v>
+        <f t="shared" si="5"/>
+        <v>5.7129581477999158</v>
       </c>
       <c r="D47">
-        <f t="shared" si="2"/>
-        <v>7.0173986126343495</v>
+        <f t="shared" si="6"/>
+        <v>7.3682685432660664</v>
       </c>
       <c r="E47">
-        <f t="shared" si="3"/>
-        <v>12.458311134348556</v>
-      </c>
-      <c r="G47">
-        <f>C47*($D$4*$E$4*EXP(-1*$E$4*$A47))</f>
-        <v>0.35947213682616602</v>
-      </c>
-      <c r="H47">
-        <f>D47*($D$4*$E$4*EXP(-1*$E$4*$A47))</f>
-        <v>0.46362797861155258</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="4"/>
-        <v>0.82310011543771866</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="5"/>
-        <v>0.13169601847003498</v>
+        <f t="shared" si="7"/>
+        <v>13.081226691065982</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="10"/>
+        <v>0.10377518046865104</v>
+      </c>
+      <c r="H47" s="3">
+        <f t="shared" si="11"/>
+        <v>0.13384368973775659</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="12"/>
+        <v>0.23761887020640765</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="13"/>
+        <v>3.8019019233025225E-2</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>